<commit_message>
[fix] substring index of fusion rules
</commit_message>
<xml_diff>
--- a/test/performance/experiment-results-new.xlsx
+++ b/test/performance/experiment-results-new.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28260" windowHeight="12480" activeTab="3"/>
+    <workbookView windowWidth="31900" windowHeight="16760" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="90">
   <si>
     <t>Example</t>
   </si>
@@ -953,7 +953,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -965,12 +965,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -990,6 +984,9 @@
     <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -998,9 +995,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1011,17 +1005,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4057,6 +4045,11 @@
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext uri="{0b15fc19-7d7d-44ad-8c2d-2c3a37ce22c3}">
+        <chartProps xmlns="https://web.wps.cn/et/2018/main" chartId="{6da9b8eb-2a05-47ef-9ebe-8d168d8ca3dd}"/>
+      </c:ext>
+    </c:extLst>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -5063,6 +5056,11 @@
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext uri="{0b15fc19-7d7d-44ad-8c2d-2c3a37ce22c3}">
+        <chartProps xmlns="https://web.wps.cn/et/2018/main" chartId="{b41a63e3-e8ca-4657-8e22-1adbfb2d310b}"/>
+      </c:ext>
+    </c:extLst>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -5753,6 +5751,11 @@
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext uri="{0b15fc19-7d7d-44ad-8c2d-2c3a37ce22c3}">
+        <chartProps xmlns="https://web.wps.cn/et/2018/main" chartId="{ecd1da5f-5e4f-4743-955c-6af80980bb14}"/>
+      </c:ext>
+    </c:extLst>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -5766,6 +5769,691 @@
           <a:alpha val="25000"/>
         </a:schemeClr>
       </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="zh-CN"/>
+      </a:pPr>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'optimized 18-ops'!$AM$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1o</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'optimized 18-ops'!$AN$10:$AV$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2-ops</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4-ops</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6-ops</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8-ops</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10-ops</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12-ops</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14-ops</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16-ops</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18-ops</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'optimized 18-ops'!$AN$11:$AV$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00_ </c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>53.88</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>79.98</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>115.99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>114.38</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>179.57</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>233.32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>262.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>355.94</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>260.14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'optimized 18-ops'!$AM$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2o</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'optimized 18-ops'!$AN$10:$AV$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2-ops</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4-ops</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6-ops</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8-ops</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10-ops</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12-ops</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14-ops</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16-ops</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18-ops</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'optimized 18-ops'!$AN$12:$AV$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00_ </c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>510.12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>539.07</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>562.53</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>540.66</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>542.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>444.61</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>442.83</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>505.96</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>441.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'optimized 18-ops'!$AM$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3o</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'optimized 18-ops'!$AN$10:$AV$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2-ops</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4-ops</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6-ops</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8-ops</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10-ops</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12-ops</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14-ops</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16-ops</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18-ops</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'optimized 18-ops'!$AN$13:$AV$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00_ </c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>700.67</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>714.15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>752.48</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>775.91</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>809.02</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>899.68</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>900.68</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1036.18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1066.37</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'optimized 18-ops'!$AM$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4o</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'optimized 18-ops'!$AN$10:$AV$10</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2-ops</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4-ops</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6-ops</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8-ops</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10-ops</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12-ops</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14-ops</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16-ops</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18-ops</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'optimized 18-ops'!$AN$14:$AV$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00_ </c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>936.17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>985.54</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1205.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1282.23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1424.16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1795.68</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1767.31</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2041.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2160.02</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="572406654"/>
+        <c:axId val="775583195"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="572406654"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1" forceAA="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+                <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+                <a:cs typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+                <a:sym typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="775583195"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="775583195"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00_ " sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1" forceAA="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+                <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+                <a:cs typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+                <a:sym typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="572406654"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1" forceAA="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:cs typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:sym typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -6067,6 +6755,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="10055">
   <cs:axisTitle>
@@ -9144,6 +9872,512 @@
 </file>
 
 <file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="10055">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst/>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst/>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="90200"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="10055">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9861,6 +11095,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>90170</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>211455</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>58</xdr:col>
+      <xdr:colOff>184785</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>208280</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="图表 1" descr="7b0a202020202263686172745265734964223a20223230343638363533220a7d0a"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="38071425" y="1278255"/>
+        <a:ext cx="5581015" cy="3197225"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -11092,6 +12356,250 @@
 </a:themeOverride>
 </file>
 
+<file path=xl/theme/themeOverride5.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="WPS">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="44546A"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="E7E6E6"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4874CB"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="EE822F"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="F2BA02"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="75BD42"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="30C0B4"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="E54C5E"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0026E5"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="7E1FAD"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="WPS">
+    <a:majorFont>
+      <a:latin typeface="Calibri Light"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="WPS">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:lumOff val="17500"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr"/>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="2700000" scaled="0"/>
+      </a:gradFill>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:hueOff val="-2520000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr"/>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="2700000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:hueOff val="-4200000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="2700000" scaled="1"/>
+        </a:gradFill>
+        <a:prstDash val="solid"/>
+        <a:miter lim="800000"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="101600" dist="50800" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:schemeClr val="phClr">
+              <a:alpha val="60000"/>
+            </a:schemeClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:reflection stA="50000" endA="300" endPos="40000" dist="25400" dir="5400000" sy="-100000" algn="bl" rotWithShape="0"/>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="63000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:tint val="95000"/>
+          <a:satMod val="170000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="93000"/>
+              <a:satMod val="150000"/>
+              <a:shade val="98000"/>
+              <a:lumMod val="102000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="50000">
+            <a:schemeClr val="phClr">
+              <a:tint val="98000"/>
+              <a:satMod val="130000"/>
+              <a:shade val="90000"/>
+              <a:lumMod val="103000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="63000"/>
+              <a:satMod val="120000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="5400000" scaled="0"/>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
@@ -11116,53 +12624,53 @@
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1" spans="1:11">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20" t="s">
+      <c r="E1" s="17"/>
+      <c r="F1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
     </row>
     <row r="2" ht="34" spans="1:14">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
       <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20" t="s">
+      <c r="G2" s="17"/>
+      <c r="H2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20" t="s">
+      <c r="I2" s="17"/>
+      <c r="J2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="20"/>
+      <c r="K2" s="17"/>
       <c r="N2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
       <c r="C3" t="s">
         <v>8</v>
       </c>
@@ -11195,10 +12703,10 @@
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="17">
         <v>22</v>
       </c>
       <c r="C4">
@@ -11233,8 +12741,8 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
       <c r="C5">
         <v>4.695731</v>
       </c>
@@ -11267,8 +12775,8 @@
       </c>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
       <c r="C6">
         <v>4.877195</v>
       </c>
@@ -11304,10 +12812,10 @@
       </c>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="17">
         <v>98</v>
       </c>
       <c r="C7">
@@ -11342,8 +12850,8 @@
       </c>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
       <c r="C8">
         <v>9.207653</v>
       </c>
@@ -11376,8 +12884,8 @@
       </c>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
       <c r="C9">
         <v>9.449012</v>
       </c>
@@ -11410,10 +12918,10 @@
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="20">
+      <c r="B10" s="17">
         <v>75</v>
       </c>
       <c r="C10">
@@ -11445,8 +12953,8 @@
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="14"/>
-      <c r="B11" s="20"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="17"/>
       <c r="C11">
         <v>7.463528</v>
       </c>
@@ -11476,8 +12984,8 @@
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="14"/>
-      <c r="B12" s="20"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="17"/>
       <c r="C12">
         <v>7.725575</v>
       </c>
@@ -11507,10 +13015,10 @@
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="20">
+      <c r="B13" s="17">
         <v>132</v>
       </c>
       <c r="C13">
@@ -11542,8 +13050,8 @@
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
       <c r="C14">
         <v>8.282757</v>
       </c>
@@ -11573,8 +13081,8 @@
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
       <c r="C15">
         <v>8.366628</v>
       </c>
@@ -11604,10 +13112,10 @@
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="20">
+      <c r="B16" s="17">
         <v>63</v>
       </c>
       <c r="C16">
@@ -11639,8 +13147,8 @@
       </c>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
       <c r="C17">
         <v>7.612231</v>
       </c>
@@ -11670,8 +13178,8 @@
       </c>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
       <c r="C18">
         <v>7.090666</v>
       </c>
@@ -11747,54 +13255,54 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="1" ht="30" customHeight="1" spans="1:11">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20" t="s">
+      <c r="E1" s="17"/>
+      <c r="F1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
     </row>
     <row r="2" customFormat="1" ht="34" spans="1:11">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
       <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20" t="s">
+      <c r="G2" s="17"/>
+      <c r="H2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20" t="s">
+      <c r="I2" s="17"/>
+      <c r="J2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="20"/>
+      <c r="K2" s="17"/>
     </row>
     <row r="3" customFormat="1" spans="1:11">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
       <c r="D3" t="s">
         <v>9</v>
       </c>
@@ -11821,7 +13329,7 @@
       </c>
     </row>
     <row r="4" customFormat="1" ht="17" spans="1:11">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B4">
@@ -11856,7 +13364,7 @@
       </c>
     </row>
     <row r="5" customFormat="1" ht="17" spans="1:11">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B5">
@@ -11891,7 +13399,7 @@
       </c>
     </row>
     <row r="6" ht="34" spans="1:11">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B6">
@@ -11926,7 +13434,7 @@
       </c>
     </row>
     <row r="7" ht="17" spans="1:11">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B7">
@@ -11961,7 +13469,7 @@
       </c>
     </row>
     <row r="8" ht="17" spans="1:11">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B8">
@@ -11996,134 +13504,134 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
     </row>
     <row r="10" customFormat="1" spans="1:5">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
     </row>
     <row r="11" customFormat="1" spans="1:5">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
     </row>
     <row r="12" customFormat="1" spans="1:5">
-      <c r="A12" s="23"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
     </row>
     <row r="13" customFormat="1" spans="1:5">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
     </row>
     <row r="14" customFormat="1" spans="1:5">
-      <c r="A14" s="23"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
     </row>
     <row r="15" customFormat="1" spans="1:5">
-      <c r="A15" s="23"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
     </row>
     <row r="16" customFormat="1" spans="1:5">
-      <c r="A16" s="23"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
     </row>
     <row r="17" customFormat="1" spans="1:5">
-      <c r="A17" s="23"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
     </row>
     <row r="18" customFormat="1" spans="1:5">
-      <c r="A18" s="23"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="23"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20" t="s">
+      <c r="E22" s="17"/>
+      <c r="F22" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
     </row>
     <row r="23" ht="34" spans="1:11">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
       <c r="D23" t="s">
         <v>4</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20" t="s">
+      <c r="G23" s="17"/>
+      <c r="H23" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20" t="s">
+      <c r="I23" s="17"/>
+      <c r="J23" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="K23" s="20"/>
+      <c r="K23" s="17"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="20"/>
-      <c r="B24" s="20"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="17"/>
       <c r="C24" t="s">
         <v>8</v>
       </c>
@@ -12153,7 +13661,7 @@
       </c>
     </row>
     <row r="25" ht="17" spans="1:11">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B25">
@@ -12188,7 +13696,7 @@
       </c>
     </row>
     <row r="26" ht="17" spans="1:11">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B26">
@@ -12223,7 +13731,7 @@
       </c>
     </row>
     <row r="27" ht="34" spans="1:11">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B27">
@@ -12258,7 +13766,7 @@
       </c>
     </row>
     <row r="28" ht="17" spans="1:11">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B28">
@@ -12293,7 +13801,7 @@
       </c>
     </row>
     <row r="29" ht="17" spans="1:11">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B29">
@@ -12395,27 +13903,27 @@
       </c>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="13"/>
-      <c r="G6" s="13"/>
+      <c r="B6" s="12"/>
+      <c r="G6" s="12"/>
     </row>
     <row r="7" ht="17" spans="2:18">
-      <c r="B7" s="14"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="1" t="s">
         <v>0</v>
       </c>
@@ -12431,7 +13939,7 @@
       <c r="G7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="7" t="s">
         <v>23</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -12461,10 +13969,10 @@
       <c r="Q7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="R7" s="20"/>
+      <c r="R7" s="17"/>
     </row>
     <row r="8" spans="2:18">
-      <c r="B8" s="14"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="1" t="s">
         <v>33</v>
       </c>
@@ -12510,10 +14018,10 @@
       <c r="Q8" s="2">
         <v>5417.181</v>
       </c>
-      <c r="R8" s="20"/>
+      <c r="R8" s="17"/>
     </row>
     <row r="9" spans="2:18">
-      <c r="B9" s="14"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -12551,10 +14059,10 @@
       <c r="Q9" s="2">
         <v>5879.29</v>
       </c>
-      <c r="R9" s="20"/>
+      <c r="R9" s="17"/>
     </row>
     <row r="10" spans="2:18">
-      <c r="B10" s="14"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -12592,10 +14100,10 @@
       <c r="Q10" s="2">
         <v>5481.19</v>
       </c>
-      <c r="R10" s="20"/>
+      <c r="R10" s="17"/>
     </row>
     <row r="11" spans="2:18">
-      <c r="B11" s="14"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="1" t="s">
         <v>38</v>
       </c>
@@ -12641,10 +14149,10 @@
       <c r="Q11" s="2">
         <v>1533.481</v>
       </c>
-      <c r="R11" s="20"/>
+      <c r="R11" s="17"/>
     </row>
     <row r="12" spans="2:18">
-      <c r="B12" s="14"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -12682,10 +14190,10 @@
       <c r="Q12" s="2">
         <v>1620.14</v>
       </c>
-      <c r="R12" s="20"/>
+      <c r="R12" s="17"/>
     </row>
     <row r="13" spans="2:18">
-      <c r="B13" s="14"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -12723,10 +14231,10 @@
       <c r="Q13" s="2">
         <v>1551.44</v>
       </c>
-      <c r="R13" s="20"/>
+      <c r="R13" s="17"/>
     </row>
     <row r="14" spans="2:18">
-      <c r="B14" s="14"/>
+      <c r="B14" s="13"/>
       <c r="C14" s="1" t="s">
         <v>40</v>
       </c>
@@ -12772,10 +14280,10 @@
       <c r="Q14" s="2">
         <v>31600.479</v>
       </c>
-      <c r="R14" s="20"/>
+      <c r="R14" s="17"/>
     </row>
     <row r="15" spans="2:18">
-      <c r="B15" s="14"/>
+      <c r="B15" s="13"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -12813,10 +14321,10 @@
       <c r="Q15" s="2">
         <v>43849.744</v>
       </c>
-      <c r="R15" s="20"/>
+      <c r="R15" s="17"/>
     </row>
     <row r="16" spans="2:18">
-      <c r="B16" s="14"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -12854,10 +14362,10 @@
       <c r="Q16" s="2">
         <v>34377.03</v>
       </c>
-      <c r="R16" s="20"/>
+      <c r="R16" s="17"/>
     </row>
     <row r="17" spans="2:18">
-      <c r="B17" s="14"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="1" t="s">
         <v>42</v>
       </c>
@@ -12903,10 +14411,10 @@
       <c r="Q17" s="2">
         <v>136322.758</v>
       </c>
-      <c r="R17" s="20"/>
+      <c r="R17" s="17"/>
     </row>
     <row r="18" spans="2:18">
-      <c r="B18" s="14"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -12944,10 +14452,10 @@
       <c r="Q18" s="2">
         <v>144968.54</v>
       </c>
-      <c r="R18" s="20"/>
+      <c r="R18" s="17"/>
     </row>
     <row r="19" spans="2:18">
-      <c r="B19" s="14"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -12985,35 +14493,35 @@
       <c r="Q19" s="2">
         <v>139031</v>
       </c>
-      <c r="R19" s="20"/>
+      <c r="R19" s="17"/>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
     </row>
     <row r="22" spans="2:2">
-      <c r="B22" s="13"/>
+      <c r="B22" s="12"/>
     </row>
     <row r="23" spans="2:2">
-      <c r="B23" s="13"/>
+      <c r="B23" s="12"/>
     </row>
     <row r="24" spans="2:2">
-      <c r="B24" s="13"/>
+      <c r="B24" s="12"/>
     </row>
     <row r="25" spans="2:12">
-      <c r="B25" s="13"/>
-      <c r="C25" s="15" t="s">
+      <c r="B25" s="12"/>
+      <c r="C25" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -13045,7 +14553,7 @@
       </c>
     </row>
     <row r="26" spans="3:12">
-      <c r="C26" s="16">
+      <c r="C26" s="14">
         <v>1</v>
       </c>
       <c r="D26" s="2">
@@ -13077,7 +14585,7 @@
       </c>
     </row>
     <row r="27" spans="3:13">
-      <c r="C27" s="16">
+      <c r="C27" s="14">
         <v>2</v>
       </c>
       <c r="D27" s="2">
@@ -13107,10 +14615,10 @@
       <c r="L27" s="2">
         <v>1551.44</v>
       </c>
-      <c r="M27" s="7"/>
+      <c r="M27" s="5"/>
     </row>
     <row r="28" spans="3:13">
-      <c r="C28" s="15">
+      <c r="C28" s="8">
         <v>3</v>
       </c>
       <c r="D28" s="2">
@@ -13143,7 +14651,7 @@
       <c r="M28" s="2"/>
     </row>
     <row r="29" spans="3:12">
-      <c r="C29" s="15">
+      <c r="C29" s="8">
         <v>4</v>
       </c>
       <c r="D29" s="2">
@@ -13175,19 +14683,19 @@
       </c>
     </row>
     <row r="30" ht="20.4" spans="2:2">
-      <c r="B30" s="17"/>
+      <c r="B30" s="15"/>
     </row>
     <row r="34" spans="2:2">
-      <c r="B34" s="18"/>
+      <c r="B34" s="16"/>
     </row>
     <row r="35" spans="2:2">
-      <c r="B35" s="18"/>
+      <c r="B35" s="16"/>
     </row>
     <row r="39" spans="2:2">
-      <c r="B39" s="18"/>
+      <c r="B39" s="16"/>
     </row>
     <row r="42" spans="2:2">
-      <c r="B42" s="18"/>
+      <c r="B42" s="16"/>
     </row>
     <row r="46" spans="4:5">
       <c r="D46" t="s">
@@ -13198,7 +14706,7 @@
       </c>
     </row>
     <row r="47" spans="2:5">
-      <c r="B47" s="18"/>
+      <c r="B47" s="16"/>
       <c r="D47">
         <v>160</v>
       </c>
@@ -13231,19 +14739,19 @@
       </c>
     </row>
     <row r="57" spans="2:2">
-      <c r="B57" s="18"/>
+      <c r="B57" s="16"/>
     </row>
     <row r="59" ht="20.4" spans="2:2">
-      <c r="B59" s="17"/>
+      <c r="B59" s="15"/>
     </row>
     <row r="61" spans="2:2">
-      <c r="B61" s="18"/>
+      <c r="B61" s="16"/>
     </row>
     <row r="62" spans="2:2">
-      <c r="B62" s="18"/>
+      <c r="B62" s="16"/>
     </row>
     <row r="63" spans="2:21">
-      <c r="B63" s="19"/>
+      <c r="B63" s="4"/>
       <c r="C63" s="1" t="s">
         <v>22</v>
       </c>
@@ -13285,7 +14793,7 @@
       <c r="U63" s="1"/>
     </row>
     <row r="64" ht="17" spans="2:21">
-      <c r="B64" s="19"/>
+      <c r="B64" s="4"/>
       <c r="C64" s="1"/>
       <c r="D64" s="2" t="s">
         <v>54</v>
@@ -13343,7 +14851,7 @@
       </c>
     </row>
     <row r="65" spans="2:21">
-      <c r="B65" s="19"/>
+      <c r="B65" s="4"/>
       <c r="C65" s="1" t="s">
         <v>35</v>
       </c>
@@ -13403,7 +14911,7 @@
       </c>
     </row>
     <row r="66" spans="2:21">
-      <c r="B66" s="19"/>
+      <c r="B66" s="4"/>
       <c r="C66" s="1" t="s">
         <v>36</v>
       </c>
@@ -13463,45 +14971,45 @@
       </c>
     </row>
     <row r="67" spans="4:20">
-      <c r="D67" s="7"/>
-      <c r="E67" s="22"/>
-      <c r="F67" s="7"/>
-      <c r="G67" s="22"/>
-      <c r="H67" s="7"/>
-      <c r="I67" s="22"/>
-      <c r="J67" s="7"/>
-      <c r="K67" s="22"/>
-      <c r="L67" s="7"/>
-      <c r="M67" s="22"/>
-      <c r="N67" s="7"/>
-      <c r="O67" s="22"/>
-      <c r="P67" s="7"/>
-      <c r="Q67" s="22"/>
-      <c r="R67" s="7"/>
-      <c r="S67" s="22"/>
-      <c r="T67" s="7"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="6"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="6"/>
+      <c r="J67" s="5"/>
+      <c r="K67" s="6"/>
+      <c r="L67" s="5"/>
+      <c r="M67" s="6"/>
+      <c r="N67" s="5"/>
+      <c r="O67" s="6"/>
+      <c r="P67" s="5"/>
+      <c r="Q67" s="6"/>
+      <c r="R67" s="5"/>
+      <c r="S67" s="6"/>
+      <c r="T67" s="5"/>
     </row>
     <row r="68" spans="4:20">
-      <c r="D68" s="7"/>
-      <c r="E68" s="22"/>
-      <c r="F68" s="7"/>
-      <c r="G68" s="22"/>
-      <c r="H68" s="7"/>
-      <c r="I68" s="22"/>
-      <c r="J68" s="7"/>
-      <c r="K68" s="22"/>
-      <c r="L68" s="7"/>
-      <c r="M68" s="22"/>
-      <c r="N68" s="7"/>
-      <c r="O68" s="22"/>
-      <c r="P68" s="7"/>
-      <c r="Q68" s="22"/>
-      <c r="R68" s="7"/>
-      <c r="S68" s="22"/>
-      <c r="T68" s="7"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="6"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="6"/>
+      <c r="J68" s="5"/>
+      <c r="K68" s="6"/>
+      <c r="L68" s="5"/>
+      <c r="M68" s="6"/>
+      <c r="N68" s="5"/>
+      <c r="O68" s="6"/>
+      <c r="P68" s="5"/>
+      <c r="Q68" s="6"/>
+      <c r="R68" s="5"/>
+      <c r="S68" s="6"/>
+      <c r="T68" s="5"/>
     </row>
     <row r="71" spans="3:21">
-      <c r="C71" s="15" t="s">
+      <c r="C71" s="8" t="s">
         <v>54</v>
       </c>
       <c r="D71" s="2">
@@ -13560,7 +15068,7 @@
       </c>
     </row>
     <row r="72" ht="17" spans="3:21">
-      <c r="C72" s="15" t="s">
+      <c r="C72" s="8" t="s">
         <v>55</v>
       </c>
       <c r="D72" s="1" t="s">
@@ -13619,91 +15127,91 @@
       </c>
     </row>
     <row r="94" ht="20.4" spans="2:2">
-      <c r="B94" s="17"/>
+      <c r="B94" s="15"/>
     </row>
     <row r="96" spans="2:13">
-      <c r="B96" s="21"/>
-      <c r="C96" s="21"/>
-      <c r="D96" s="21"/>
-      <c r="E96" s="21"/>
-      <c r="F96" s="21"/>
-      <c r="G96" s="21"/>
-      <c r="H96" s="21"/>
-      <c r="I96" s="21"/>
-      <c r="J96" s="21"/>
-      <c r="K96" s="21"/>
-      <c r="L96" s="21"/>
-      <c r="M96" s="21"/>
+      <c r="B96" s="18"/>
+      <c r="C96" s="18"/>
+      <c r="D96" s="18"/>
+      <c r="E96" s="18"/>
+      <c r="F96" s="18"/>
+      <c r="G96" s="18"/>
+      <c r="H96" s="18"/>
+      <c r="I96" s="18"/>
+      <c r="J96" s="18"/>
+      <c r="K96" s="18"/>
+      <c r="L96" s="18"/>
+      <c r="M96" s="18"/>
     </row>
     <row r="97" spans="2:13">
-      <c r="B97" s="13"/>
-      <c r="C97" s="13"/>
-      <c r="D97" s="13"/>
-      <c r="E97" s="13"/>
-      <c r="F97" s="13"/>
-      <c r="G97" s="13"/>
-      <c r="H97" s="13"/>
-      <c r="I97" s="13"/>
-      <c r="J97" s="13"/>
-      <c r="K97" s="13"/>
-      <c r="L97" s="13"/>
-      <c r="M97" s="13"/>
+      <c r="B97" s="12"/>
+      <c r="C97" s="12"/>
+      <c r="D97" s="12"/>
+      <c r="E97" s="12"/>
+      <c r="F97" s="12"/>
+      <c r="G97" s="12"/>
+      <c r="H97" s="12"/>
+      <c r="I97" s="12"/>
+      <c r="J97" s="12"/>
+      <c r="K97" s="12"/>
+      <c r="L97" s="12"/>
+      <c r="M97" s="12"/>
     </row>
     <row r="98" spans="2:13">
-      <c r="B98" s="13"/>
-      <c r="C98" s="13"/>
-      <c r="D98" s="13"/>
-      <c r="E98" s="13"/>
-      <c r="F98" s="13"/>
-      <c r="G98" s="13"/>
-      <c r="H98" s="13"/>
-      <c r="I98" s="13"/>
-      <c r="J98" s="13"/>
-      <c r="K98" s="13"/>
-      <c r="L98" s="13"/>
-      <c r="M98" s="13"/>
+      <c r="B98" s="12"/>
+      <c r="C98" s="12"/>
+      <c r="D98" s="12"/>
+      <c r="E98" s="12"/>
+      <c r="F98" s="12"/>
+      <c r="G98" s="12"/>
+      <c r="H98" s="12"/>
+      <c r="I98" s="12"/>
+      <c r="J98" s="12"/>
+      <c r="K98" s="12"/>
+      <c r="L98" s="12"/>
+      <c r="M98" s="12"/>
     </row>
     <row r="99" spans="2:13">
-      <c r="B99" s="13"/>
-      <c r="C99" s="13"/>
-      <c r="D99" s="13"/>
-      <c r="E99" s="13"/>
-      <c r="F99" s="13"/>
-      <c r="G99" s="13"/>
-      <c r="H99" s="13"/>
-      <c r="I99" s="13"/>
-      <c r="J99" s="13"/>
-      <c r="K99" s="13"/>
-      <c r="L99" s="13"/>
-      <c r="M99" s="13"/>
+      <c r="B99" s="12"/>
+      <c r="C99" s="12"/>
+      <c r="D99" s="12"/>
+      <c r="E99" s="12"/>
+      <c r="F99" s="12"/>
+      <c r="G99" s="12"/>
+      <c r="H99" s="12"/>
+      <c r="I99" s="12"/>
+      <c r="J99" s="12"/>
+      <c r="K99" s="12"/>
+      <c r="L99" s="12"/>
+      <c r="M99" s="12"/>
     </row>
     <row r="100" spans="2:13">
-      <c r="B100" s="13"/>
-      <c r="C100" s="13"/>
-      <c r="D100" s="13"/>
-      <c r="E100" s="13"/>
-      <c r="F100" s="13"/>
-      <c r="G100" s="13"/>
-      <c r="H100" s="13"/>
-      <c r="I100" s="13"/>
-      <c r="J100" s="13"/>
-      <c r="K100" s="13"/>
-      <c r="L100" s="13"/>
-      <c r="M100" s="13"/>
+      <c r="B100" s="12"/>
+      <c r="C100" s="12"/>
+      <c r="D100" s="12"/>
+      <c r="E100" s="12"/>
+      <c r="F100" s="12"/>
+      <c r="G100" s="12"/>
+      <c r="H100" s="12"/>
+      <c r="I100" s="12"/>
+      <c r="J100" s="12"/>
+      <c r="K100" s="12"/>
+      <c r="L100" s="12"/>
+      <c r="M100" s="12"/>
     </row>
     <row r="101" spans="2:13">
-      <c r="B101" s="13"/>
-      <c r="C101" s="13"/>
-      <c r="D101" s="13"/>
-      <c r="E101" s="13"/>
-      <c r="F101" s="13"/>
-      <c r="G101" s="13"/>
-      <c r="H101" s="13"/>
-      <c r="I101" s="13"/>
-      <c r="J101" s="13"/>
-      <c r="K101" s="13"/>
-      <c r="L101" s="13"/>
-      <c r="M101" s="13"/>
+      <c r="B101" s="12"/>
+      <c r="C101" s="12"/>
+      <c r="D101" s="12"/>
+      <c r="E101" s="12"/>
+      <c r="F101" s="12"/>
+      <c r="G101" s="12"/>
+      <c r="H101" s="12"/>
+      <c r="I101" s="12"/>
+      <c r="J101" s="12"/>
+      <c r="K101" s="12"/>
+      <c r="L101" s="12"/>
+      <c r="M101" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="28">
@@ -13745,10 +15253,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B2:AQ46"/>
+  <dimension ref="B2:AV46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="157" zoomScaleNormal="157" topLeftCell="J27" workbookViewId="0">
-      <selection activeCell="M37" sqref="M37"/>
+    <sheetView tabSelected="1" zoomScale="157" zoomScaleNormal="157" topLeftCell="AT3" workbookViewId="0">
+      <selection activeCell="BC24" sqref="BC24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8"/>
@@ -13817,19 +15325,19 @@
       <c r="O2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AM2" s="5" t="s">
+      <c r="AM2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AN2" s="5" t="s">
+      <c r="AN2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AO2" s="5" t="s">
+      <c r="AO2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AP2" s="5" t="s">
+      <c r="AP2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AQ2" s="5" t="s">
+      <c r="AQ2" s="1" t="s">
         <v>76</v>
       </c>
     </row>
@@ -13876,19 +15384,19 @@
       <c r="O3" s="2">
         <v>243.38</v>
       </c>
-      <c r="AM3" s="5">
+      <c r="AM3" s="1">
         <v>1</v>
       </c>
-      <c r="AN3" s="5" t="s">
+      <c r="AN3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AO3" s="5" t="s">
+      <c r="AO3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AP3" s="5" t="s">
+      <c r="AP3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AQ3" s="5" t="s">
+      <c r="AQ3" s="1" t="s">
         <v>78</v>
       </c>
     </row>
@@ -13921,25 +15429,25 @@
       <c r="M4" s="2">
         <v>548.94</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="9">
         <v>874.97</v>
       </c>
       <c r="O4" s="2">
         <v>321.61</v>
       </c>
-      <c r="AM4" s="5">
+      <c r="AM4" s="1">
         <v>2</v>
       </c>
-      <c r="AN4" s="5" t="s">
+      <c r="AN4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AO4" s="5" t="s">
+      <c r="AO4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AP4" s="5" t="s">
+      <c r="AP4" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AQ4" s="12" t="s">
+      <c r="AQ4" s="11" t="s">
         <v>80</v>
       </c>
     </row>
@@ -13978,19 +15486,19 @@
       <c r="O5" s="2">
         <v>260.14</v>
       </c>
-      <c r="AM5" s="5">
+      <c r="AM5" s="1">
         <v>3</v>
       </c>
-      <c r="AN5" s="5" t="s">
+      <c r="AN5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AO5" s="5" t="s">
+      <c r="AO5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AP5" s="5" t="s">
+      <c r="AP5" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AQ5" s="5" t="s">
+      <c r="AQ5" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -14037,19 +15545,19 @@
       <c r="O6" s="2">
         <v>432.28</v>
       </c>
-      <c r="AM6" s="5">
+      <c r="AM6" s="1">
         <v>4</v>
       </c>
-      <c r="AN6" s="5" t="s">
+      <c r="AN6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AO6" s="5" t="s">
+      <c r="AO6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AP6" s="5" t="s">
+      <c r="AP6" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AQ6" s="5" t="s">
+      <c r="AQ6" s="1" t="s">
         <v>84</v>
       </c>
     </row>
@@ -14169,7 +15677,7 @@
         <v>1048.57</v>
       </c>
     </row>
-    <row r="10" spans="2:37">
+    <row r="10" spans="2:48">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -14204,7 +15712,7 @@
       <c r="O10" s="2">
         <v>1123.23</v>
       </c>
-      <c r="AB10" s="4" t="s">
+      <c r="AB10" s="1" t="s">
         <v>0</v>
       </c>
       <c r="AC10" s="1" t="s">
@@ -14234,8 +15742,38 @@
       <c r="AK10" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="AM10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AO10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AQ10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AR10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AS10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AT10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AU10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AV10" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="11" spans="2:37">
+    <row r="11" spans="2:48">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -14270,7 +15808,7 @@
       <c r="O11" s="2">
         <v>1066.37</v>
       </c>
-      <c r="AB11" s="9">
+      <c r="AB11" s="7">
         <v>1</v>
       </c>
       <c r="AC11" s="2">
@@ -14300,8 +15838,38 @@
       <c r="AK11" s="2">
         <v>5481.19</v>
       </c>
+      <c r="AM11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AN11" s="2">
+        <v>53.88</v>
+      </c>
+      <c r="AO11" s="2">
+        <v>79.98</v>
+      </c>
+      <c r="AP11" s="2">
+        <v>115.99</v>
+      </c>
+      <c r="AQ11" s="2">
+        <v>114.38</v>
+      </c>
+      <c r="AR11" s="2">
+        <v>179.57</v>
+      </c>
+      <c r="AS11" s="2">
+        <v>233.32</v>
+      </c>
+      <c r="AT11" s="2">
+        <v>262.25</v>
+      </c>
+      <c r="AU11" s="2">
+        <v>355.94</v>
+      </c>
+      <c r="AV11" s="2">
+        <v>260.14</v>
+      </c>
     </row>
-    <row r="12" spans="2:37">
+    <row r="12" spans="2:48">
       <c r="B12" s="1" t="s">
         <v>42</v>
       </c>
@@ -14344,7 +15912,7 @@
       <c r="O12" s="2">
         <v>2136.41</v>
       </c>
-      <c r="AB12" s="5" t="s">
+      <c r="AB12" s="1" t="s">
         <v>85</v>
       </c>
       <c r="AC12" s="2">
@@ -14374,8 +15942,38 @@
       <c r="AK12" s="2">
         <v>260.14</v>
       </c>
+      <c r="AM12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN12" s="2">
+        <v>510.12</v>
+      </c>
+      <c r="AO12" s="2">
+        <v>539.07</v>
+      </c>
+      <c r="AP12" s="2">
+        <v>562.53</v>
+      </c>
+      <c r="AQ12" s="2">
+        <v>540.66</v>
+      </c>
+      <c r="AR12" s="2">
+        <v>542.7</v>
+      </c>
+      <c r="AS12" s="2">
+        <v>444.61</v>
+      </c>
+      <c r="AT12" s="2">
+        <v>442.83</v>
+      </c>
+      <c r="AU12" s="2">
+        <v>505.96</v>
+      </c>
+      <c r="AV12" s="2">
+        <v>441.99</v>
+      </c>
     </row>
-    <row r="13" spans="2:37">
+    <row r="13" spans="2:48">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -14410,7 +16008,7 @@
       <c r="O13" s="2">
         <v>2240.27</v>
       </c>
-      <c r="AB13" s="9">
+      <c r="AB13" s="7">
         <v>2</v>
       </c>
       <c r="AC13" s="2">
@@ -14440,8 +16038,38 @@
       <c r="AK13" s="2">
         <v>1551.44</v>
       </c>
+      <c r="AM13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN13" s="2">
+        <v>700.67</v>
+      </c>
+      <c r="AO13" s="2">
+        <v>714.15</v>
+      </c>
+      <c r="AP13" s="2">
+        <v>752.48</v>
+      </c>
+      <c r="AQ13" s="2">
+        <v>775.91</v>
+      </c>
+      <c r="AR13" s="2">
+        <v>809.02</v>
+      </c>
+      <c r="AS13" s="2">
+        <v>899.68</v>
+      </c>
+      <c r="AT13" s="2">
+        <v>900.68</v>
+      </c>
+      <c r="AU13" s="2">
+        <v>1036.18</v>
+      </c>
+      <c r="AV13" s="2">
+        <v>1066.37</v>
+      </c>
     </row>
-    <row r="14" spans="2:37">
+    <row r="14" spans="2:48">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -14476,7 +16104,7 @@
       <c r="O14" s="2">
         <v>2160.02</v>
       </c>
-      <c r="AB14" s="5" t="s">
+      <c r="AB14" s="1" t="s">
         <v>86</v>
       </c>
       <c r="AC14" s="2">
@@ -14506,9 +16134,39 @@
       <c r="AK14" s="2">
         <v>441.99</v>
       </c>
+      <c r="AM14" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AN14" s="2">
+        <v>936.17</v>
+      </c>
+      <c r="AO14" s="2">
+        <v>985.54</v>
+      </c>
+      <c r="AP14" s="2">
+        <v>1205.01</v>
+      </c>
+      <c r="AQ14" s="2">
+        <v>1282.23</v>
+      </c>
+      <c r="AR14" s="2">
+        <v>1424.16</v>
+      </c>
+      <c r="AS14" s="2">
+        <v>1795.68</v>
+      </c>
+      <c r="AT14" s="2">
+        <v>1767.31</v>
+      </c>
+      <c r="AU14" s="2">
+        <v>2041.4</v>
+      </c>
+      <c r="AV14" s="2">
+        <v>2160.02</v>
+      </c>
     </row>
-    <row r="15" spans="28:37">
-      <c r="AB15" s="4">
+    <row r="15" spans="28:48">
+      <c r="AB15" s="1">
         <v>3</v>
       </c>
       <c r="AC15" s="2">
@@ -14538,9 +16196,19 @@
       <c r="AK15" s="2">
         <v>34377.03</v>
       </c>
+      <c r="AM15" s="4"/>
+      <c r="AN15" s="5"/>
+      <c r="AO15" s="5"/>
+      <c r="AP15" s="5"/>
+      <c r="AQ15" s="5"/>
+      <c r="AR15" s="5"/>
+      <c r="AS15" s="5"/>
+      <c r="AT15" s="5"/>
+      <c r="AU15" s="5"/>
+      <c r="AV15" s="5"/>
     </row>
-    <row r="16" spans="28:37">
-      <c r="AB16" s="5" t="s">
+    <row r="16" spans="28:48">
+      <c r="AB16" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC16" s="2">
@@ -14570,9 +16238,19 @@
       <c r="AK16" s="2">
         <v>1066.37</v>
       </c>
+      <c r="AM16" s="10"/>
+      <c r="AN16" s="10"/>
+      <c r="AO16" s="10"/>
+      <c r="AP16" s="10"/>
+      <c r="AQ16" s="10"/>
+      <c r="AR16" s="10"/>
+      <c r="AS16" s="10"/>
+      <c r="AT16" s="10"/>
+      <c r="AU16" s="10"/>
+      <c r="AV16" s="10"/>
     </row>
-    <row r="17" spans="6:37">
-      <c r="F17" s="4" t="s">
+    <row r="17" spans="6:48">
+      <c r="F17" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G17" s="1" t="s">
@@ -14602,7 +16280,7 @@
       <c r="O17" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AB17" s="4">
+      <c r="AB17" s="1">
         <v>4</v>
       </c>
       <c r="AC17" s="2">
@@ -14632,9 +16310,19 @@
       <c r="AK17" s="2">
         <v>139031</v>
       </c>
+      <c r="AM17" s="4"/>
+      <c r="AN17" s="5"/>
+      <c r="AO17" s="5"/>
+      <c r="AP17" s="5"/>
+      <c r="AQ17" s="5"/>
+      <c r="AR17" s="5"/>
+      <c r="AS17" s="5"/>
+      <c r="AT17" s="5"/>
+      <c r="AU17" s="5"/>
+      <c r="AV17" s="5"/>
     </row>
     <row r="18" spans="6:37">
-      <c r="F18" s="9">
+      <c r="F18" s="7">
         <v>1</v>
       </c>
       <c r="G18" s="2">
@@ -14664,7 +16352,7 @@
       <c r="O18" s="2">
         <v>5481.19</v>
       </c>
-      <c r="AB18" s="5" t="s">
+      <c r="AB18" s="1" t="s">
         <v>88</v>
       </c>
       <c r="AC18" s="2">
@@ -14696,7 +16384,7 @@
       </c>
     </row>
     <row r="19" spans="6:15">
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="1" t="s">
         <v>85</v>
       </c>
       <c r="G19" s="2">
@@ -14728,7 +16416,7 @@
       </c>
     </row>
     <row r="20" spans="6:15">
-      <c r="F20" s="9">
+      <c r="F20" s="7">
         <v>2</v>
       </c>
       <c r="G20" s="2">
@@ -14760,7 +16448,7 @@
       </c>
     </row>
     <row r="21" spans="6:15">
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="1" t="s">
         <v>86</v>
       </c>
       <c r="G21" s="2">
@@ -14792,7 +16480,7 @@
       </c>
     </row>
     <row r="23" spans="6:15">
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G23" s="1" t="s">
@@ -14824,7 +16512,7 @@
       </c>
     </row>
     <row r="24" spans="6:15">
-      <c r="F24" s="4">
+      <c r="F24" s="1">
         <v>3</v>
       </c>
       <c r="G24" s="2">
@@ -14856,7 +16544,7 @@
       </c>
     </row>
     <row r="25" spans="6:15">
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="1" t="s">
         <v>87</v>
       </c>
       <c r="G25" s="2">
@@ -14888,7 +16576,7 @@
       </c>
     </row>
     <row r="26" spans="6:15">
-      <c r="F26" s="4">
+      <c r="F26" s="1">
         <v>4</v>
       </c>
       <c r="G26" s="2">
@@ -14920,7 +16608,7 @@
       </c>
     </row>
     <row r="27" spans="6:15">
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="1" t="s">
         <v>88</v>
       </c>
       <c r="G27" s="2">
@@ -15062,7 +16750,7 @@
       <c r="E34" s="1">
         <v>1</v>
       </c>
-      <c r="F34" s="10">
+      <c r="F34" s="8">
         <v>4</v>
       </c>
       <c r="G34" s="1">
@@ -15074,37 +16762,37 @@
       <c r="I34" s="1">
         <v>2</v>
       </c>
-      <c r="J34" s="10">
+      <c r="J34" s="8">
         <v>1</v>
       </c>
       <c r="K34" s="1">
         <v>2</v>
       </c>
-      <c r="L34" s="10">
+      <c r="L34" s="8">
         <v>1</v>
       </c>
       <c r="M34" s="1">
         <v>4</v>
       </c>
-      <c r="N34" s="10">
+      <c r="N34" s="8">
         <v>2</v>
       </c>
       <c r="O34" s="1">
         <v>4</v>
       </c>
-      <c r="P34" s="10">
+      <c r="P34" s="8">
         <v>2</v>
       </c>
       <c r="Q34" s="3">
         <v>8</v>
       </c>
-      <c r="R34" s="10">
+      <c r="R34" s="8">
         <v>1</v>
       </c>
       <c r="S34" s="1">
         <v>256</v>
       </c>
-      <c r="T34" s="10">
+      <c r="T34" s="8">
         <v>4</v>
       </c>
     </row>
@@ -15121,7 +16809,7 @@
       <c r="E35" s="1">
         <v>64</v>
       </c>
-      <c r="F35" s="10">
+      <c r="F35" s="8">
         <v>4</v>
       </c>
       <c r="G35" s="1">
@@ -15133,42 +16821,42 @@
       <c r="I35" s="1">
         <v>256</v>
       </c>
-      <c r="J35" s="10">
+      <c r="J35" s="8">
         <v>8</v>
       </c>
       <c r="K35" s="1">
         <v>768</v>
       </c>
-      <c r="L35" s="10">
+      <c r="L35" s="8">
         <v>8</v>
       </c>
       <c r="M35" s="1">
         <v>768</v>
       </c>
-      <c r="N35" s="10">
+      <c r="N35" s="8">
         <v>8</v>
       </c>
       <c r="O35" s="1">
         <v>768</v>
       </c>
-      <c r="P35" s="10">
+      <c r="P35" s="8">
         <v>8</v>
       </c>
       <c r="Q35" s="2">
         <v>768</v>
       </c>
-      <c r="R35" s="10">
+      <c r="R35" s="8">
         <v>8</v>
       </c>
       <c r="S35" s="1">
         <v>256</v>
       </c>
-      <c r="T35" s="10">
+      <c r="T35" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="39" spans="2:11">
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -15200,7 +16888,7 @@
       </c>
     </row>
     <row r="40" spans="2:11">
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C40" s="2">
@@ -15232,7 +16920,7 @@
       </c>
     </row>
     <row r="41" spans="2:11">
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C41" s="2">
@@ -15264,7 +16952,7 @@
       </c>
     </row>
     <row r="42" spans="2:11">
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C42" s="2">
@@ -15296,7 +16984,7 @@
       </c>
     </row>
     <row r="43" spans="2:11">
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C43" s="2">
@@ -15328,40 +17016,40 @@
       </c>
     </row>
     <row r="44" spans="2:11">
-      <c r="B44" s="6"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="7"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
     </row>
     <row r="45" spans="2:11">
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="8"/>
-      <c r="K45" s="8"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="6"/>
     </row>
     <row r="46" spans="2:11">
-      <c r="B46" s="6"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="7"/>
-      <c r="K46" s="7"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="26">

</xml_diff>